<commit_message>
added more data points
</commit_message>
<xml_diff>
--- a/data/places_aayushi_visited.xlsx
+++ b/data/places_aayushi_visited.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushiverma/Documents/Github/world-exploration-map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushiverma/Documents/Github/world-exploration-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE1633C-50ED-3349-851E-7BBB27EB5086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9EA2E9-C4FD-7D40-A3DD-806C8F4EB6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="19340" xr2:uid="{A76A3374-AE1A-B54F-972B-2CBFACF199FD}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="18980" windowHeight="19340" xr2:uid="{A76A3374-AE1A-B54F-972B-2CBFACF199FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>Country</t>
   </si>
@@ -288,6 +288,27 @@
   </si>
   <si>
     <t>Missisauga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA </t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>I really only transit through LAX, I don't think I've ever actally stepped foot in LA…</t>
+  </si>
+  <si>
+    <t>Rotorua</t>
+  </si>
+  <si>
+    <t>Bay of Plenty</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Tasman</t>
   </si>
 </sst>
 </file>
@@ -640,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E30941-C829-6340-A053-D17F5B08A40A}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,6 +1345,51 @@
         <v>44986</v>
       </c>
     </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="1">
+        <v>44621</v>
+      </c>
+      <c r="F45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="1">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="1">
+        <v>42339</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F41">
     <sortCondition ref="A1:A41"/>

</xml_diff>

<commit_message>
updated data and data source
now using live google Sheets instead of static Excel, but still need to save as a .hyper
</commit_message>
<xml_diff>
--- a/data/places_aayushi_visited.xlsx
+++ b/data/places_aayushi_visited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aayushiverma/Documents/Github/world-exploration-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C763C946-E923-B446-A832-BB66403799B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3F6F3D-F716-6045-B41C-CB3FDC6E996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="500" windowWidth="34000" windowHeight="19320" xr2:uid="{A76A3374-AE1A-B54F-972B-2CBFACF199FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="138">
   <si>
     <t>Country</t>
   </si>
@@ -420,6 +420,36 @@
   </si>
   <si>
     <t>Visited Kennedy Space Center here!</t>
+  </si>
+  <si>
+    <t>Mansfield</t>
+  </si>
+  <si>
+    <t>Hartford</t>
+  </si>
+  <si>
+    <t>South Windsor</t>
+  </si>
+  <si>
+    <t>Visited University of Connecticut here! It's a very beautiful campus!</t>
+  </si>
+  <si>
+    <t>Stayed at Cambria Hotel Manchester South Windsor here, it's a bougie hotel without the bougie price tag!</t>
+  </si>
+  <si>
+    <t>Nice downtown area.</t>
+  </si>
+  <si>
+    <t>Port Deposit</t>
+  </si>
+  <si>
+    <t>Stopped at Chesapeake Travel Plaza - bougie rest area!</t>
+  </si>
+  <si>
+    <t>College Park</t>
+  </si>
+  <si>
+    <t>Visited University of Maryland campus!</t>
   </si>
 </sst>
 </file>
@@ -772,11 +802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E30941-C829-6340-A053-D17F5B08A40A}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,7 +1515,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="1">
-        <v>45261</v>
+        <v>45323</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>116</v>
@@ -1544,6 +1574,9 @@
       <c r="C38" t="s">
         <v>55</v>
       </c>
+      <c r="D38" s="1">
+        <v>43405</v>
+      </c>
       <c r="E38" s="1">
         <v>44652</v>
       </c>
@@ -1585,7 +1618,7 @@
         <v>47</v>
       </c>
       <c r="E40" s="1">
-        <v>43466</v>
+        <v>45375</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>115</v>
@@ -2029,6 +2062,121 @@
       </c>
       <c r="G62" s="1" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D63" s="1">
+        <v>45352</v>
+      </c>
+      <c r="E63" s="1">
+        <v>45352</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="1">
+        <v>45352</v>
+      </c>
+      <c r="E64" s="1">
+        <v>45352</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="1">
+        <v>45352</v>
+      </c>
+      <c r="E65" s="1">
+        <v>45352</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45352</v>
+      </c>
+      <c r="E66" s="1">
+        <v>45352</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="1">
+        <v>45323</v>
+      </c>
+      <c r="E67" s="1">
+        <v>45323</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>